<commit_message>
Updated naming convension for columns
</commit_message>
<xml_diff>
--- a/tbemr_basicRegister_codebook_v1.0.xlsx
+++ b/tbemr_basicRegister_codebook_v1.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kristina.reinhardt\OneDrive - MSF\EMR\_tbemr\tbemr_metabase_queries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kristina.reinhardt\OneDrive - MSF\EMR\bahmni-mart\5_queryLibrary\mart-tbemr-query-library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80A5C41-E62F-4492-AAC7-416EE105032B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A70B04-E069-4320-B79C-439CA1B0571A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A005DB92-A8DC-40CC-A3FD-38C99E047FDE}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">basic_register_description!$A$1:$J$65</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="287">
   <si>
     <t>Column</t>
   </si>
@@ -88,9 +90,6 @@
     <t>n/a</t>
   </si>
   <si>
-    <t>Register</t>
-  </si>
-  <si>
     <t>Name of register patient belongs to (either BMU or Secondline TB)</t>
   </si>
   <si>
@@ -106,9 +105,6 @@
     <t>Second-line TB treatment register; Basic Management Unit TB register</t>
   </si>
   <si>
-    <t>EMR ID</t>
-  </si>
-  <si>
     <t>EMR auto-generated ID assigned to patient at registration</t>
   </si>
   <si>
@@ -124,9 +120,6 @@
     <t>patient id</t>
   </si>
   <si>
-    <t>Sex</t>
-  </si>
-  <si>
     <t>Sex of patient</t>
   </si>
   <si>
@@ -181,9 +174,6 @@
     <t>New; relapse; treatment after loss to followup; treatment after failure; other previously treated patients</t>
   </si>
   <si>
-    <t>History of Previously Treated</t>
-  </si>
-  <si>
     <t>Baseline form &gt; Case Definition section &gt; Previously treated group</t>
   </si>
   <si>
@@ -193,9 +183,6 @@
     <t>Previously treated with first line drugs only; previously treated with second line drugs; histroy unclear/unknown</t>
   </si>
   <si>
-    <t>MTB Confirmed</t>
-  </si>
-  <si>
     <t>Baseline form &gt; Case Definition section &gt; MTB Confirmation</t>
   </si>
   <si>
@@ -221,9 +208,6 @@
   </si>
   <si>
     <t>H(S) resistance; HE(S) resistance; R resistance with H susceptibility; GeneXpert RIF resistance only; Confirmed MDR; Confirmed pre-XDR (FQ); Confirmed pre-XDR (Inj); Confirmed XDR; Other</t>
-  </si>
-  <si>
-    <t>Treatment Start Date</t>
   </si>
   <si>
     <t>Treatment Initiation form &gt; Treatment Initiation section &gt; Treatment Start Date</t>
@@ -270,9 +254,6 @@
     <t>coded drug name = 'Bedaquiline (Bdq)' and earliest start date</t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
     <t>Isoniazid (H) is part of initial TB drug regimen</t>
   </si>
   <si>
@@ -285,141 +266,72 @@
     <t>If drug was started and then stopped by accident, then drug will still appear as part of the initial drug regimen</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
     <t>Rifampicin (R) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>Ethambutol (E) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>Z</t>
-  </si>
-  <si>
     <t>Pyrazinamide (Z) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>Streptomycin (S) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>Am</t>
-  </si>
-  <si>
     <t>Amikacin (Am) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>Km</t>
-  </si>
-  <si>
     <t>Kanamycin (Km) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>Cm</t>
-  </si>
-  <si>
     <t>Capreomycin (Cm) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>Lfx</t>
-  </si>
-  <si>
     <t>Levofloxacin (Lfx) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>Mfx</t>
-  </si>
-  <si>
     <t>Moxifloxacin (Mfx) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>Pto</t>
-  </si>
-  <si>
     <t>Prothionamide (Pto) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>Eto</t>
-  </si>
-  <si>
     <t>Ethionamide (Eto) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>Cs</t>
-  </si>
-  <si>
     <t>Cycloserine (Cs) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>Trd</t>
-  </si>
-  <si>
     <t>Terizidone (Trd) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>PAS</t>
-  </si>
-  <si>
     <t>Para-aminosalicylic acid (PAS) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>PAS-Na</t>
-  </si>
-  <si>
     <t>Para-aminosalicylic acid-sodium (PAS-Na) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>Bdq</t>
-  </si>
-  <si>
     <t>Bedaquiline (Bdq) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>Dlm</t>
-  </si>
-  <si>
     <t>Delamanid (Dlm) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>Lzd</t>
-  </si>
-  <si>
     <t>Linezolid (Lzd) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>Cfz</t>
-  </si>
-  <si>
     <t>Clofazimine (Cfz) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>Imp/Clm</t>
-  </si>
-  <si>
     <t>Imipenem/Cilastatin (Imp/Clm) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>Amx/Clv</t>
-  </si>
-  <si>
     <t>Amoxicillin/Clavulanate (Amx/Clv) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>Mpm</t>
-  </si>
-  <si>
     <t>Meropenem (Mpm) is part of initial TB drug regimen</t>
   </si>
   <si>
-    <t>HIV Baseline</t>
-  </si>
-  <si>
     <t>Baseline form &gt; Past Medical History section &gt; HIV &gt; Baseline HIV</t>
   </si>
   <si>
@@ -448,9 +360,6 @@
   </si>
   <si>
     <t>This value is going to be continuosly changing for patients who are still receiving treatment and having new HIV tests added to their patient file</t>
-  </si>
-  <si>
-    <t>HIV Status</t>
   </si>
   <si>
     <t>Summary of HIV baseline and lab results - providing the last known HIV status of patient</t>
@@ -467,9 +376,6 @@
     <t>Lab Hiv Test Result; HIV serostatus result</t>
   </si>
   <si>
-    <t>Hep B Baseline</t>
-  </si>
-  <si>
     <t>Baseline form &gt; Past Medical History section &gt; Hepatitis &gt; Hepatitis B</t>
   </si>
   <si>
@@ -489,9 +395,6 @@
   </si>
   <si>
     <t>This value is going to be continuosly changing for patients who are still receiving treatment and having new hepatitis tests added to their patient file</t>
-  </si>
-  <si>
-    <t>Hep B Status</t>
   </si>
   <si>
     <t>Summary of Hep B baseline and lab results - providing the last known Hep B status of patient</t>
@@ -508,9 +411,6 @@
     <t xml:space="preserve">If lab test is 'borderline' or 'pending' or baseline status was 'unknown', these will not show up - only the most recent positive/negative results. </t>
   </si>
   <si>
-    <t>Hep C Baseline</t>
-  </si>
-  <si>
     <t>Baseline form &gt; Past Medical History section &gt; Hepatitis &gt; Hepatitis C</t>
   </si>
   <si>
@@ -524,9 +424,6 @@
   </si>
   <si>
     <t xml:space="preserve">Lab Hepatitis C Antibody Test Result </t>
-  </si>
-  <si>
-    <t>Hep C Status</t>
   </si>
   <si>
     <t>Summary of Hep C baseline and lab results - providing the last known Hep C status of patient</t>
@@ -540,16 +437,10 @@
     <t>Lab Hepatitis C Antibody Test Result; Baseline hepatitis C</t>
   </si>
   <si>
-    <t>Diabetes Baseline</t>
-  </si>
-  <si>
     <t>Baseline form &gt; Past Medical History section &gt; Chronic diseases sub-section &gt; Diabetes</t>
   </si>
   <si>
     <t>Diabetes mellitus</t>
-  </si>
-  <si>
-    <t>Outcome</t>
   </si>
   <si>
     <t>Outcome - End of Treatment Form &gt; Outcome</t>
@@ -623,18 +514,6 @@
     <t>Added two start date variables. 1) Earliest start date of either Dlm or Bdq; and 2) start date if Dlm and Bdq were started within one week of each other.</t>
   </si>
   <si>
-    <t>Start Date (Dlm)</t>
-  </si>
-  <si>
-    <t>Start Date (Bdq)</t>
-  </si>
-  <si>
-    <t>Start Date (Dlm or Bdq)</t>
-  </si>
-  <si>
-    <t>Start Date (Dlm and Bdq)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Date the patient first started either Dlm or Bdq. </t>
   </si>
   <si>
@@ -650,9 +529,6 @@
     <t>Changed HIV status codes to 'HIV Positive'/'HIV Negative' from 'Positive'/'Negative'</t>
   </si>
   <si>
-    <t>Baseline Disease Site</t>
-  </si>
-  <si>
     <t>Baseline form &gt; Case Definition section &gt; Disease Site</t>
   </si>
   <si>
@@ -671,9 +547,6 @@
     <t>Added secondline treatment type from treatment initiation form</t>
   </si>
   <si>
-    <t>Second line treatment type</t>
-  </si>
-  <si>
     <t>Treatment Initiation form &gt; Treatment Initiation section &gt; Second line treatment type</t>
   </si>
   <si>
@@ -773,12 +646,6 @@
     <t>Added Initial Culture Conversion, months to initial culture conversion and positive culture after initial culture conversion variables</t>
   </si>
   <si>
-    <t>Initial Culture Conversion Date</t>
-  </si>
-  <si>
-    <t>Months to Initial Culture Conversion</t>
-  </si>
-  <si>
     <t>numeric</t>
   </si>
   <si>
@@ -830,12 +697,6 @@
     <t xml:space="preserve">If no facility is mentioned in any of the three forms, the registration facility from program enrollment is used. If "Other" facility has been selected on the hospital admission notification form or follow-up form, then the free text name of the facility is used. </t>
   </si>
   <si>
-    <t>Pa</t>
-  </si>
-  <si>
-    <t>Rpt or P</t>
-  </si>
-  <si>
     <t>Rifapentine (Rpt or P) is part of initial TB drug regimen</t>
   </si>
   <si>
@@ -848,45 +709,9 @@
     <t xml:space="preserve">The next visit date from the most recent follow-up form.If there is any follow-up form completed, the next visit date if from the most recent form, even if null. If there is follow-up form completed, then the next visit date is from the baseline template form. </t>
   </si>
   <si>
-    <t>Registration Number</t>
-  </si>
-  <si>
-    <t>Age at Registration</t>
-  </si>
-  <si>
-    <t>Age group at Registration</t>
-  </si>
-  <si>
-    <t>WHO Registration Group</t>
-  </si>
-  <si>
-    <t>Drug Resistance Profile</t>
-  </si>
-  <si>
-    <t>Sub-class of Drug Resistance Profile</t>
-  </si>
-  <si>
-    <t>Treatment Duration (months)</t>
-  </si>
-  <si>
-    <t>Last Facility</t>
-  </si>
-  <si>
     <t>Last reported treatment facility from treatment initiation, hospital admission notification and follow-up forms. If no recent facility is mentioned, the registration facility from program enrollment is displayed.</t>
   </si>
   <si>
-    <t>HIV Lab</t>
-  </si>
-  <si>
-    <t>Hep B Lab</t>
-  </si>
-  <si>
-    <t>Hep C Lab</t>
-  </si>
-  <si>
-    <t>Positive Culture at Baseline</t>
-  </si>
-  <si>
     <t>Diabetes status at baseline</t>
   </si>
   <si>
@@ -896,28 +721,214 @@
     <t>Does not take negative culture results into account</t>
   </si>
   <si>
-    <t xml:space="preserve">Negative Culture Closer to Baseline Than Positive Culture </t>
-  </si>
-  <si>
     <t xml:space="preserve">Indication if patient had a negative culture result closer to treatment start date than a positive culture result. Only patients with a positive culture result either up to 90 days before or 15 days after the treatment start date are considered. </t>
   </si>
   <si>
     <t xml:space="preserve">Only patients with a positive culture result either up to 90 days before or 15 days after the treatment start date are considered. </t>
   </si>
   <si>
-    <t>Culture Conversion (for positive at baseline only)</t>
-  </si>
-  <si>
     <t>Y,N,null</t>
   </si>
   <si>
     <t>Indication of patients who had a positive culture result at baseline who have cultured converted. 'Y' for positive culture result at baseline and have culture convered and 'N' for positive culture result at baseline but have not culture converted.</t>
   </si>
   <si>
-    <t>Re-conversion after Initial Culture Conversion</t>
-  </si>
-  <si>
     <t>Integrated additional culture conversion variables.</t>
+  </si>
+  <si>
+    <t>Renamed column names (added numbering) to adjust for Metabase automatic alphabetical ordering in v0.31 and v0.34</t>
+  </si>
+  <si>
+    <t>02_Register</t>
+  </si>
+  <si>
+    <t>01_Registration_Number</t>
+  </si>
+  <si>
+    <t>04_Sex</t>
+  </si>
+  <si>
+    <t>05_Age_at_Registration</t>
+  </si>
+  <si>
+    <t>07_WHO_Registration_Group</t>
+  </si>
+  <si>
+    <t>08_History_of_Previously_Treated</t>
+  </si>
+  <si>
+    <t>10_MTB_Confirmed</t>
+  </si>
+  <si>
+    <t>11_Drug_Resistance_Profile</t>
+  </si>
+  <si>
+    <t>12_Sub-class_of_Drug_Resistance_Profile</t>
+  </si>
+  <si>
+    <t>13_Treatment_Start_Date</t>
+  </si>
+  <si>
+    <t>14_Treatment_Duration_(months)</t>
+  </si>
+  <si>
+    <t>16_Start_Date_(Dlm)</t>
+  </si>
+  <si>
+    <t>17_Start_Date_(Bdq)</t>
+  </si>
+  <si>
+    <t>18_Start_Date_(Dlm_or_Bdq)</t>
+  </si>
+  <si>
+    <t>19_Start_Date_(Dlm_and_Bdq)</t>
+  </si>
+  <si>
+    <t>20_Last_Facility</t>
+  </si>
+  <si>
+    <t>46_HIV_Baseline</t>
+  </si>
+  <si>
+    <t>47_HIV_Lab</t>
+  </si>
+  <si>
+    <t>48_HIV_Status</t>
+  </si>
+  <si>
+    <t>49_Hep_B_Baseline</t>
+  </si>
+  <si>
+    <t>50_Hep_B_Lab</t>
+  </si>
+  <si>
+    <t>51_Hep_B_Status</t>
+  </si>
+  <si>
+    <t>52_Hep_C_Baseline</t>
+  </si>
+  <si>
+    <t>53_Hep_C_Lab</t>
+  </si>
+  <si>
+    <t>54_Hep_C_Status</t>
+  </si>
+  <si>
+    <t>55_Diabetes_Baseline</t>
+  </si>
+  <si>
+    <t>56_Positive_Culture_at_Baseline</t>
+  </si>
+  <si>
+    <t>58_Culture_Conversion_(for_positive_at_baseline_only)</t>
+  </si>
+  <si>
+    <t>59_Initial_Culture_Conversion_Date</t>
+  </si>
+  <si>
+    <t>60_Months_to_Initial_Culture_Conversion</t>
+  </si>
+  <si>
+    <t>62_Outcome</t>
+  </si>
+  <si>
+    <t>09_Baseline_Disease_Site</t>
+  </si>
+  <si>
+    <t>63_End_of_Treatment_Date</t>
+  </si>
+  <si>
+    <t>57_Negative_Culture_Closer_to_Baseline_Than_Positive_Culture</t>
+  </si>
+  <si>
+    <t>21_Initial_Drug_H</t>
+  </si>
+  <si>
+    <t>22_Initial_Drug_R</t>
+  </si>
+  <si>
+    <t>23_Initial_Drug_E</t>
+  </si>
+  <si>
+    <t>24_Initial_Drug_Z</t>
+  </si>
+  <si>
+    <t>25_Initial_Drug_S</t>
+  </si>
+  <si>
+    <t>26_Initial_Drug_Am</t>
+  </si>
+  <si>
+    <t>27_Initial_Drug_Km</t>
+  </si>
+  <si>
+    <t>28_Initial_Drug_Cm</t>
+  </si>
+  <si>
+    <t>29_Initial_Drug_Lfx</t>
+  </si>
+  <si>
+    <t>30_Initial_Drug_Mfx</t>
+  </si>
+  <si>
+    <t>31_Initial_Drug_Pto</t>
+  </si>
+  <si>
+    <t>32_Initial_Drug_Eto</t>
+  </si>
+  <si>
+    <t>33_Initial_Drug_Cs</t>
+  </si>
+  <si>
+    <t>34_Initial_Drug_Trd</t>
+  </si>
+  <si>
+    <t>35_Initial_Drug_PAS</t>
+  </si>
+  <si>
+    <t>36_Initial_Drug_PAS-Na</t>
+  </si>
+  <si>
+    <t>37_Initial_Drug_Bdq</t>
+  </si>
+  <si>
+    <t>38_Initial_Drug_Dlm</t>
+  </si>
+  <si>
+    <t>39_Initial_Drug_Lzd</t>
+  </si>
+  <si>
+    <t>40_Initial_Drug_Cfz</t>
+  </si>
+  <si>
+    <t>41_Initial_Drug_Imp/Clm</t>
+  </si>
+  <si>
+    <t>42_Initial_Drug_Amx/Clv</t>
+  </si>
+  <si>
+    <t>43_Initial_Drug_Mpm</t>
+  </si>
+  <si>
+    <t>44_Initial_Drug_Pa</t>
+  </si>
+  <si>
+    <t>45_Initial_Drug_Rpt_or_P</t>
+  </si>
+  <si>
+    <t>06_Age_Group_at_Registration</t>
+  </si>
+  <si>
+    <t>03_EMR_ID</t>
+  </si>
+  <si>
+    <t>64_Next_Visit</t>
+  </si>
+  <si>
+    <t>61_Reconversion_after_Initial_Culture_Conversion</t>
+  </si>
+  <si>
+    <t>15_Second_Line_Treatment_Type</t>
   </si>
 </sst>
 </file>
@@ -979,7 +990,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1093,7 +1104,48 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1106,7 +1158,9 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1119,7 +1173,9 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1132,12 +1188,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1147,12 +1201,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1162,19 +1214,17 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1200,35 +1250,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1237,6 +1263,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1553,10 +1606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AFB7678-3E18-497F-ABA7-7D2FE6D40AA7}">
-  <dimension ref="B1:D15"/>
+  <dimension ref="B1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1569,80 +1622,80 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>182</v>
+      <c r="B2" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B3" s="9">
+      <c r="B3" s="17">
         <v>43521</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>183</v>
+      <c r="C3" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="5">
         <v>43521</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>193</v>
+      <c r="C4" s="9" t="s">
+        <v>152</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>183</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" s="5">
         <v>43521</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>199</v>
+      <c r="C5" s="9" t="s">
+        <v>157</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>183</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="5">
         <v>43521</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>200</v>
+      <c r="C6" s="10" t="s">
+        <v>158</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>183</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="5">
         <v>43521</v>
       </c>
-      <c r="C7" s="16" t="s">
-        <v>224</v>
+      <c r="C7" s="10" t="s">
+        <v>181</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>183</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" s="5">
         <v>43521</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>225</v>
+      <c r="C8" s="10" t="s">
+        <v>182</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>183</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
@@ -1650,10 +1703,10 @@
         <v>43782</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>232</v>
+        <v>189</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>183</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
@@ -1661,10 +1714,10 @@
         <v>43782</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>233</v>
+        <v>190</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>183</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1672,10 +1725,10 @@
         <v>43784</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>234</v>
+        <v>191</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>183</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
@@ -1683,26 +1736,57 @@
         <v>43832</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>283</v>
+        <v>221</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="7"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="2:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="2:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="5">
+        <v>44074</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="5"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="20"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
+    </row>
+    <row r="16" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="20"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="22"/>
+    </row>
+    <row r="17" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="20"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="22"/>
+    </row>
+    <row r="18" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="20"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="22"/>
+    </row>
+    <row r="19" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="22"/>
+    </row>
+    <row r="20" spans="2:4" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="7"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="8"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:D8">
@@ -1717,59 +1801,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{755CC844-63E2-4B85-BD9F-12E3C1EFFCA3}">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17" style="19" customWidth="1"/>
-    <col min="2" max="2" width="33" style="19" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" style="19" customWidth="1"/>
-    <col min="4" max="6" width="27" style="19" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="19" customWidth="1"/>
-    <col min="8" max="9" width="23" style="19" customWidth="1"/>
-    <col min="10" max="10" width="49.109375" style="19" customWidth="1"/>
-    <col min="11" max="16384" width="8.6640625" style="19"/>
+    <col min="1" max="1" width="46" style="11" customWidth="1"/>
+    <col min="2" max="2" width="33" style="11" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" style="11" customWidth="1"/>
+    <col min="4" max="6" width="27" style="11" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="11" customWidth="1"/>
+    <col min="8" max="9" width="23" style="11" customWidth="1"/>
+    <col min="10" max="10" width="49.109375" style="11" customWidth="1"/>
+    <col min="11" max="16384" width="8.6640625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="21" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:10" s="13" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="42" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>260</v>
+        <v>224</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
@@ -1796,56 +1880,56 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="69" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="I3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>230</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>15</v>
@@ -1859,57 +1943,57 @@
     </row>
     <row r="5" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="F5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="I5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>261</v>
+        <v>226</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>205</v>
+        <v>162</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>16</v>
@@ -1920,28 +2004,28 @@
     </row>
     <row r="7" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>16</v>
@@ -1949,28 +2033,28 @@
     </row>
     <row r="8" spans="1:10" s="2" customFormat="1" ht="69" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>206</v>
+        <v>163</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="G8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>16</v>
@@ -1978,28 +2062,28 @@
     </row>
     <row r="9" spans="1:10" s="2" customFormat="1" ht="69" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>48</v>
+        <v>228</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>207</v>
+        <v>164</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>16</v>
@@ -2007,28 +2091,28 @@
     </row>
     <row r="10" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>194</v>
+        <v>254</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>209</v>
+        <v>166</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>195</v>
+        <v>153</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>196</v>
+        <v>154</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>197</v>
+        <v>155</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>198</v>
+        <v>156</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>16</v>
@@ -2036,28 +2120,28 @@
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>52</v>
+        <v>229</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>210</v>
+        <v>167</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>16</v>
@@ -2065,28 +2149,28 @@
     </row>
     <row r="12" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>264</v>
+        <v>230</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>208</v>
+        <v>165</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>16</v>
@@ -2094,28 +2178,28 @@
     </row>
     <row r="13" spans="1:10" s="2" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>265</v>
+        <v>231</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>211</v>
+        <v>168</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>16</v>
@@ -2123,54 +2207,54 @@
     </row>
     <row r="14" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>62</v>
+        <v>232</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>212</v>
+        <v>169</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="2" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>266</v>
+        <v>233</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>215</v>
+        <v>172</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>237</v>
+        <v>192</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>16</v>
@@ -2179,33 +2263,33 @@
         <v>16</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>213</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="2" customFormat="1" ht="151.80000000000001" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>201</v>
+        <v>286</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>214</v>
+        <v>171</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>202</v>
+        <v>159</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>204</v>
+        <v>161</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>16</v>
@@ -2213,976 +2297,976 @@
     </row>
     <row r="17" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>185</v>
+        <v>234</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>220</v>
+        <v>177</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>186</v>
+        <v>235</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>220</v>
+        <v>177</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>187</v>
+        <v>236</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>189</v>
+        <v>148</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>220</v>
+        <v>177</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>190</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="2" customFormat="1" ht="69" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>188</v>
+        <v>237</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>191</v>
+        <v>150</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>220</v>
+        <v>177</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>192</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="2" customFormat="1" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>267</v>
+        <v>238</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>268</v>
+        <v>213</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>250</v>
+        <v>205</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>251</v>
+        <v>206</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>252</v>
+        <v>207</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>253</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>77</v>
+        <v>257</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>82</v>
+        <v>258</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>84</v>
+        <v>259</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>86</v>
+        <v>260</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>88</v>
+        <v>261</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>90</v>
+        <v>262</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>92</v>
+        <v>263</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>94</v>
+        <v>264</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>96</v>
+        <v>265</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>98</v>
+        <v>266</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>100</v>
+        <v>267</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>102</v>
+        <v>268</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>104</v>
+        <v>269</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>106</v>
+        <v>270</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>108</v>
+        <v>271</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>110</v>
+        <v>272</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>112</v>
+        <v>273</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>114</v>
+        <v>274</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>116</v>
+        <v>275</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>118</v>
+        <v>276</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>120</v>
+        <v>277</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>122</v>
+        <v>278</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>124</v>
+        <v>279</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>125</v>
+        <v>96</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>254</v>
+        <v>280</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>257</v>
+        <v>210</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>255</v>
+        <v>281</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>256</v>
+        <v>209</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>126</v>
+        <v>239</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>216</v>
+        <v>173</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>127</v>
+        <v>97</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>16</v>
@@ -3190,92 +3274,92 @@
     </row>
     <row r="48" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>269</v>
+        <v>240</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:10" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>137</v>
+        <v>241</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>140</v>
+        <v>109</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>141</v>
+        <v>110</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>227</v>
+        <v>184</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>142</v>
+        <v>242</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>217</v>
+        <v>174</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>16</v>
@@ -3283,92 +3367,92 @@
     </row>
     <row r="51" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>270</v>
+        <v>243</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>149</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:10" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>150</v>
+        <v>244</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>151</v>
+        <v>118</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>140</v>
+        <v>109</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>153</v>
+        <v>120</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>228</v>
+        <v>185</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>155</v>
+        <v>245</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>16</v>
@@ -3376,92 +3460,92 @@
     </row>
     <row r="54" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>271</v>
+        <v>246</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>158</v>
+        <v>124</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>159</v>
+        <v>125</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>149</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>161</v>
+        <v>247</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>140</v>
+        <v>109</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>229</v>
+        <v>186</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>165</v>
+        <v>248</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>273</v>
+        <v>214</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>166</v>
+        <v>130</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>167</v>
+        <v>131</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>226</v>
+        <v>183</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>16</v>
@@ -3469,202 +3553,202 @@
     </row>
     <row r="57" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>272</v>
+        <v>249</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>274</v>
+        <v>215</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>242</v>
+        <v>197</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>244</v>
+        <v>199</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>246</v>
+        <v>201</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>238</v>
+        <v>193</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>275</v>
+        <v>216</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>276</v>
+        <v>256</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>277</v>
+        <v>217</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>242</v>
+        <v>197</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>244</v>
+        <v>199</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>246</v>
+        <v>201</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>238</v>
+        <v>193</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>278</v>
+        <v>218</v>
       </c>
     </row>
     <row r="59" spans="1:10" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>279</v>
+        <v>250</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>281</v>
+        <v>220</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>242</v>
+        <v>197</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>244</v>
+        <v>199</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>246</v>
+        <v>201</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>280</v>
+        <v>219</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>278</v>
+        <v>218</v>
       </c>
     </row>
     <row r="60" spans="1:10" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>239</v>
+        <v>194</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>242</v>
+        <v>197</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>244</v>
+        <v>199</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>246</v>
+        <v>201</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>248</v>
+        <v>203</v>
       </c>
     </row>
     <row r="61" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>240</v>
+        <v>195</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>242</v>
+        <v>197</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>244</v>
+        <v>199</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>246</v>
+        <v>201</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>237</v>
+        <v>192</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>249</v>
+        <v>204</v>
       </c>
     </row>
     <row r="62" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>241</v>
+        <v>196</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>243</v>
+        <v>198</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>245</v>
+        <v>200</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>247</v>
+        <v>202</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>238</v>
+        <v>193</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>249</v>
+        <v>204</v>
       </c>
     </row>
     <row r="63" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>168</v>
+        <v>253</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>219</v>
+        <v>176</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>169</v>
+        <v>132</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>170</v>
+        <v>133</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>171</v>
+        <v>134</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>172</v>
+        <v>135</v>
       </c>
       <c r="I63" s="2" t="s">
         <v>16</v>
@@ -3672,25 +3756,25 @@
     </row>
     <row r="64" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>173</v>
+        <v>255</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>170</v>
+        <v>133</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>175</v>
+        <v>138</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>16</v>
@@ -3701,34 +3785,34 @@
     </row>
     <row r="65" spans="1:10" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>176</v>
+        <v>284</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>259</v>
+        <v>212</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>177</v>
+        <v>140</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>178</v>
+        <v>141</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>176</v>
+        <v>139</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I65" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J65" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="J65" s="2" t="s">
-        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>